<commit_message>
Uhhh.... A lot. Cant remember the details but added stuff to clean up test weight and also calculate lsmeans
</commit_message>
<xml_diff>
--- a/exports/yield_files/HIF 5.xlsx
+++ b/exports/yield_files/HIF 5.xlsx
@@ -5204,7 +5204,9 @@
       <c r="T83" t="n">
         <v>2.5</v>
       </c>
-      <c r="U83"/>
+      <c r="U83" t="n">
+        <v>53.9</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
@@ -5263,7 +5265,9 @@
       <c r="T84" t="n">
         <v>2.5</v>
       </c>
-      <c r="U84"/>
+      <c r="U84" t="n">
+        <v>54.2</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
@@ -5308,7 +5312,9 @@
         <v>16.3</v>
       </c>
       <c r="T85"/>
-      <c r="U85"/>
+      <c r="U85" t="n">
+        <v>54.5</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="s">

</xml_diff>